<commit_message>
made some changes to metadata and scripts
</commit_message>
<xml_diff>
--- a/data/01_pd-samples/strain_list.xlsx
+++ b/data/01_pd-samples/strain_list.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caprinapugliese/Documents/School/Uconn/2024-26_Grad_School/Dagilis-lab/WNS-project/data/01_pd-samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{03E0823C-1CB9-4245-8108-723801B9F3B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C43E28F-C8E6-B147-AFD6-69C4A1C6CD73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="1520" windowWidth="13400" windowHeight="16940" xr2:uid="{E848E2DB-0487-E946-84FD-94D9478329DB}"/>
+    <workbookView xWindow="1000" yWindow="1520" windowWidth="19160" windowHeight="14160" xr2:uid="{E848E2DB-0487-E946-84FD-94D9478329DB}"/>
   </bookViews>
   <sheets>
     <sheet name="strain_list" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="64">
   <si>
     <t>location</t>
   </si>
@@ -209,6 +222,9 @@
   </si>
   <si>
     <t>not in dataset</t>
+  </si>
+  <si>
+    <t>US Forest Service</t>
   </si>
 </sst>
 </file>
@@ -351,7 +367,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -534,6 +550,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -698,9 +720,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1100,14 +1123,14 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1305,7 +1328,7 @@
         <v>12</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="F8" s="1">
         <v>2008</v>
@@ -1315,25 +1338,25 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="D9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="2">
         <v>2008</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="2" t="s">
         <v>60</v>
       </c>
       <c r="H9" t="s">

</xml_diff>